<commit_message>
took the last value
</commit_message>
<xml_diff>
--- a/Tiempos_Escalabilidad.xlsx
+++ b/Tiempos_Escalabilidad.xlsx
@@ -151,15 +151,15 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -225,6 +225,9 @@
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>1000000</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>20088490</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>3344</v>

</xml_diff>

<commit_message>
little change in excel file
</commit_message>
<xml_diff>
--- a/Tiempos_Escalabilidad.xlsx
+++ b/Tiempos_Escalabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sami_\Desktop\SAMI\SEPTIMO SEMESTRE\ArquitecturaSoftware\SoftwareArchitecture_FraSCAti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCE3CAA-2DD7-4A84-A55D-37A13F9FD2E7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C508C11-2266-43A2-96CD-8F6A22D46C06}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t xml:space="preserve">Cada palabra es de tamaño 30. Los tiemos están tomados en milisegundos. </t>
   </si>
   <si>
-    <t xml:space="preserve">Como se puede observar en las mediciones del tiempo, shellsort es más rápido para completar la tarea a comparación del bubblesort. Esto se debe a su implementación y a sus diferencias en la complejidad temporal: en el mejor de los casos,n2 para el bubblesort y nlogn para el shellsort; en el peor de los casos, n2 para el bubblesort y n1.25 para el shellsort. En conclusión, podriamos decir que el shellsort es más escalable. </t>
+    <t xml:space="preserve">Como se puede observar en las mediciones del tiempo, shellsort es más rápido para completar la tarea a comparación del bubblesort. Esto se debe a su implementación y a sus diferencias en la complejidad temporal: en el mejor de los casos,n^2 para el bubblesort y nlogn para el shellsort; en el peor de los casos, n^2 para el bubblesort y n^1.25 para el shellsort. En conclusión, podriamos decir que el shellsort es más escalable. </t>
   </si>
 </sst>
 </file>
@@ -87,10 +87,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3850,15 +3850,15 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -3870,19 +3870,19 @@
       <c r="C2">
         <v>576</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -3894,17 +3894,17 @@
       <c r="C3">
         <v>1224</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -3916,13 +3916,13 @@
       <c r="C4">
         <v>1603</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -3934,17 +3934,17 @@
       <c r="C5">
         <v>2494</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -3956,17 +3956,17 @@
       <c r="C6">
         <v>3344</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>

</xml_diff>